<commit_message>
Changed task 1.1 and remove task for research on tools
Changed task 1.1 and remove task for research on tools
</commit_message>
<xml_diff>
--- a/Gantt chart_assign1.xlsx
+++ b/Gantt chart_assign1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9260" yWindow="8000" windowWidth="39700" windowHeight="16040" tabRatio="500"/>
+    <workbookView xWindow="10180" yWindow="3580" windowWidth="39700" windowHeight="16040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
   <si>
     <t>GANTT CHART TEMPLATE</t>
   </si>
@@ -110,90 +110,78 @@
     <phoneticPr fontId="28" type="noConversion"/>
   </si>
   <si>
+    <t>Project Definition and Planning</t>
+    <phoneticPr fontId="28" type="noConversion"/>
+  </si>
+  <si>
+    <t>S</t>
+    <phoneticPr fontId="28" type="noConversion"/>
+  </si>
+  <si>
+    <t>S</t>
+    <phoneticPr fontId="28" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPRINT ONE</t>
+    <phoneticPr fontId="28" type="noConversion"/>
+  </si>
+  <si>
+    <t>WEEK 3</t>
+    <phoneticPr fontId="28" type="noConversion"/>
+  </si>
+  <si>
+    <t>S</t>
+    <phoneticPr fontId="28" type="noConversion"/>
+  </si>
+  <si>
+    <t>Literature Review</t>
+    <phoneticPr fontId="28" type="noConversion"/>
+  </si>
+  <si>
+    <t>Research on datasets</t>
+    <phoneticPr fontId="28" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPRINT TWO</t>
+    <phoneticPr fontId="28" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPRINT THREE</t>
+    <phoneticPr fontId="28" type="noConversion"/>
+  </si>
+  <si>
+    <t>S</t>
+    <phoneticPr fontId="28" type="noConversion"/>
+  </si>
+  <si>
+    <t>WEEK 5</t>
+    <phoneticPr fontId="28" type="noConversion"/>
+  </si>
+  <si>
+    <t>WEEK 6</t>
+    <phoneticPr fontId="28" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTEM46</t>
+    <phoneticPr fontId="28" type="noConversion"/>
+  </si>
+  <si>
+    <t>Literature Review</t>
+    <phoneticPr fontId="28" type="noConversion"/>
+  </si>
+  <si>
+    <t>DELIVERABLES</t>
+    <phoneticPr fontId="28" type="noConversion"/>
+  </si>
+  <si>
     <t>Project Charter</t>
     <phoneticPr fontId="28" type="noConversion"/>
   </si>
   <si>
-    <t>Project Definition and Planning</t>
-    <phoneticPr fontId="28" type="noConversion"/>
-  </si>
-  <si>
-    <t>S</t>
-    <phoneticPr fontId="28" type="noConversion"/>
-  </si>
-  <si>
-    <t>S</t>
-    <phoneticPr fontId="28" type="noConversion"/>
-  </si>
-  <si>
-    <t>SPRINT ONE</t>
-    <phoneticPr fontId="28" type="noConversion"/>
-  </si>
-  <si>
-    <t>WEEK 3</t>
-    <phoneticPr fontId="28" type="noConversion"/>
-  </si>
-  <si>
-    <t>S</t>
-    <phoneticPr fontId="28" type="noConversion"/>
-  </si>
-  <si>
-    <t>Literature Review</t>
-    <phoneticPr fontId="28" type="noConversion"/>
-  </si>
-  <si>
-    <t>Research on datasets</t>
-    <phoneticPr fontId="28" type="noConversion"/>
-  </si>
-  <si>
-    <t>SPRINT TWO</t>
-    <phoneticPr fontId="28" type="noConversion"/>
-  </si>
-  <si>
-    <t>SPRINT THREE</t>
-    <phoneticPr fontId="28" type="noConversion"/>
-  </si>
-  <si>
-    <t>S</t>
-    <phoneticPr fontId="28" type="noConversion"/>
-  </si>
-  <si>
-    <t>WEEK 5</t>
-    <phoneticPr fontId="28" type="noConversion"/>
-  </si>
-  <si>
-    <t>WEEK 6</t>
-    <phoneticPr fontId="28" type="noConversion"/>
-  </si>
-  <si>
-    <t>CTEM46</t>
-    <phoneticPr fontId="28" type="noConversion"/>
-  </si>
-  <si>
-    <t>Literature Review</t>
-    <phoneticPr fontId="28" type="noConversion"/>
-  </si>
-  <si>
-    <t>Research on tools</t>
-    <phoneticPr fontId="28" type="noConversion"/>
-  </si>
-  <si>
-    <t>DELIVERABLES</t>
-    <phoneticPr fontId="28" type="noConversion"/>
-  </si>
-  <si>
-    <t>Project Charter</t>
-    <phoneticPr fontId="28" type="noConversion"/>
-  </si>
-  <si>
     <t>Datasets</t>
     <phoneticPr fontId="28" type="noConversion"/>
   </si>
   <si>
-    <t>Potential tools</t>
-    <phoneticPr fontId="28" type="noConversion"/>
-  </si>
-  <si>
     <t>List of Relevant Literature</t>
     <phoneticPr fontId="28" type="noConversion"/>
   </si>
@@ -203,6 +191,10 @@
   </si>
   <si>
     <t>Literature Review Report</t>
+    <phoneticPr fontId="28" type="noConversion"/>
+  </si>
+  <si>
+    <t>Problem definition</t>
     <phoneticPr fontId="28" type="noConversion"/>
   </si>
 </sst>
@@ -672,8 +664,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -879,6 +881,41 @@
     <xf numFmtId="0" fontId="29" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -898,10 +935,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -914,39 +947,8 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="31">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="已瀏覽過的超連結" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="已瀏覽過的超連結" xfId="4" builtinId="9" hidden="1"/>
@@ -958,6 +960,11 @@
     <cellStyle name="已瀏覽過的超連結" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="已瀏覽過的超連結" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="已瀏覽過的超連結" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="超連結" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超連結" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超連結" xfId="5" builtinId="8" hidden="1"/>
@@ -968,6 +975,11 @@
     <cellStyle name="超連結" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="超連結" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="超連結" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="29" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1246,10 +1258,10 @@
     <tabColor rgb="FF3D85C6"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AZ22"/>
+  <dimension ref="A1:AZ21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="AO18" sqref="AO18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
@@ -1326,48 +1338,48 @@
     </row>
     <row r="2" spans="1:52" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
-      <c r="K2" s="69" t="s">
+      <c r="K2" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="70"/>
-      <c r="S2" s="75" t="s">
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="83"/>
+      <c r="R2" s="83"/>
+      <c r="S2" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="T2" s="70"/>
-      <c r="U2" s="70"/>
-      <c r="V2" s="70"/>
-      <c r="W2" s="70"/>
-      <c r="X2" s="70"/>
-      <c r="Y2" s="70"/>
-      <c r="Z2" s="70"/>
-      <c r="AA2" s="70"/>
-      <c r="AB2" s="70"/>
-      <c r="AC2" s="70"/>
-      <c r="AD2" s="70"/>
-      <c r="AE2" s="70"/>
-      <c r="AF2" s="70"/>
-      <c r="AG2" s="70"/>
-      <c r="AH2" s="70"/>
-      <c r="AI2" s="70"/>
-      <c r="AJ2" s="70"/>
-      <c r="AK2" s="70"/>
+      <c r="T2" s="83"/>
+      <c r="U2" s="83"/>
+      <c r="V2" s="83"/>
+      <c r="W2" s="83"/>
+      <c r="X2" s="83"/>
+      <c r="Y2" s="83"/>
+      <c r="Z2" s="83"/>
+      <c r="AA2" s="83"/>
+      <c r="AB2" s="83"/>
+      <c r="AC2" s="83"/>
+      <c r="AD2" s="83"/>
+      <c r="AE2" s="83"/>
+      <c r="AF2" s="83"/>
+      <c r="AG2" s="83"/>
+      <c r="AH2" s="83"/>
+      <c r="AI2" s="83"/>
+      <c r="AJ2" s="83"/>
+      <c r="AK2" s="83"/>
       <c r="AL2" s="58"/>
       <c r="AM2" s="1"/>
       <c r="AN2" s="1"/>
@@ -1440,49 +1452,49 @@
     </row>
     <row r="4" spans="1:52" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="77" t="s">
+      <c r="C4" s="76"/>
+      <c r="D4" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
-      <c r="K4" s="72" t="s">
+      <c r="K4" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
-      <c r="N4" s="73"/>
-      <c r="O4" s="73"/>
-      <c r="P4" s="73"/>
-      <c r="Q4" s="73"/>
-      <c r="R4" s="73"/>
-      <c r="S4" s="73"/>
-      <c r="T4" s="76" t="s">
-        <v>40</v>
-      </c>
-      <c r="U4" s="73"/>
-      <c r="V4" s="73"/>
-      <c r="W4" s="73"/>
-      <c r="X4" s="73"/>
-      <c r="Y4" s="73"/>
-      <c r="Z4" s="73"/>
-      <c r="AA4" s="73"/>
-      <c r="AB4" s="73"/>
-      <c r="AC4" s="73"/>
-      <c r="AD4" s="73"/>
-      <c r="AE4" s="73"/>
-      <c r="AF4" s="73"/>
-      <c r="AG4" s="73"/>
-      <c r="AH4" s="73"/>
-      <c r="AI4" s="73"/>
-      <c r="AJ4" s="73"/>
+      <c r="L4" s="76"/>
+      <c r="M4" s="76"/>
+      <c r="N4" s="76"/>
+      <c r="O4" s="76"/>
+      <c r="P4" s="76"/>
+      <c r="Q4" s="76"/>
+      <c r="R4" s="76"/>
+      <c r="S4" s="76"/>
+      <c r="T4" s="87" t="s">
+        <v>39</v>
+      </c>
+      <c r="U4" s="76"/>
+      <c r="V4" s="76"/>
+      <c r="W4" s="76"/>
+      <c r="X4" s="76"/>
+      <c r="Y4" s="76"/>
+      <c r="Z4" s="76"/>
+      <c r="AA4" s="76"/>
+      <c r="AB4" s="76"/>
+      <c r="AC4" s="76"/>
+      <c r="AD4" s="76"/>
+      <c r="AE4" s="76"/>
+      <c r="AF4" s="76"/>
+      <c r="AG4" s="76"/>
+      <c r="AH4" s="76"/>
+      <c r="AI4" s="76"/>
+      <c r="AJ4" s="76"/>
       <c r="AK4" s="58"/>
       <c r="AL4" s="58"/>
       <c r="AM4" s="1"/>
@@ -1502,48 +1514,48 @@
     </row>
     <row r="5" spans="1:52" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="83" t="s">
+      <c r="C5" s="76"/>
+      <c r="D5" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
       <c r="J5" s="16"/>
-      <c r="K5" s="72" t="s">
+      <c r="K5" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="73"/>
-      <c r="M5" s="73"/>
-      <c r="N5" s="73"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="73"/>
-      <c r="Q5" s="73"/>
-      <c r="R5" s="73"/>
-      <c r="S5" s="73"/>
-      <c r="T5" s="74">
+      <c r="L5" s="76"/>
+      <c r="M5" s="76"/>
+      <c r="N5" s="76"/>
+      <c r="O5" s="76"/>
+      <c r="P5" s="76"/>
+      <c r="Q5" s="76"/>
+      <c r="R5" s="76"/>
+      <c r="S5" s="76"/>
+      <c r="T5" s="85">
         <v>43961</v>
       </c>
-      <c r="U5" s="73"/>
-      <c r="V5" s="73"/>
-      <c r="W5" s="73"/>
-      <c r="X5" s="73"/>
-      <c r="Y5" s="73"/>
-      <c r="Z5" s="73"/>
-      <c r="AA5" s="73"/>
-      <c r="AB5" s="73"/>
-      <c r="AC5" s="73"/>
-      <c r="AD5" s="73"/>
-      <c r="AE5" s="73"/>
-      <c r="AF5" s="73"/>
-      <c r="AG5" s="73"/>
-      <c r="AH5" s="73"/>
-      <c r="AI5" s="73"/>
+      <c r="U5" s="76"/>
+      <c r="V5" s="76"/>
+      <c r="W5" s="76"/>
+      <c r="X5" s="76"/>
+      <c r="Y5" s="76"/>
+      <c r="Z5" s="76"/>
+      <c r="AA5" s="76"/>
+      <c r="AB5" s="76"/>
+      <c r="AC5" s="76"/>
+      <c r="AD5" s="76"/>
+      <c r="AE5" s="76"/>
+      <c r="AF5" s="76"/>
+      <c r="AG5" s="76"/>
+      <c r="AH5" s="76"/>
+      <c r="AI5" s="76"/>
       <c r="AJ5" s="17"/>
       <c r="AK5" s="59"/>
       <c r="AL5" s="59"/>
@@ -1672,156 +1684,156 @@
     </row>
     <row r="8" spans="1:52" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="21"/>
-      <c r="B8" s="81" t="s">
+      <c r="B8" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="81" t="s">
+      <c r="C8" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="81" t="s">
+      <c r="D8" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="81" t="s">
+      <c r="E8" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="81" t="s">
+      <c r="F8" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="81" t="s">
+      <c r="G8" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="81" t="s">
+      <c r="H8" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="81" t="s">
-        <v>43</v>
-      </c>
-      <c r="J8" s="87" t="s">
-        <v>30</v>
-      </c>
-      <c r="K8" s="87"/>
-      <c r="L8" s="87"/>
-      <c r="M8" s="87"/>
-      <c r="N8" s="87"/>
-      <c r="O8" s="87"/>
-      <c r="P8" s="87"/>
-      <c r="Q8" s="87"/>
-      <c r="R8" s="87"/>
-      <c r="S8" s="87"/>
-      <c r="T8" s="87"/>
-      <c r="U8" s="87"/>
-      <c r="V8" s="87"/>
-      <c r="W8" s="87"/>
-      <c r="X8" s="88" t="s">
+      <c r="I8" s="65" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="73" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73"/>
+      <c r="M8" s="73"/>
+      <c r="N8" s="73"/>
+      <c r="O8" s="73"/>
+      <c r="P8" s="73"/>
+      <c r="Q8" s="73"/>
+      <c r="R8" s="73"/>
+      <c r="S8" s="73"/>
+      <c r="T8" s="73"/>
+      <c r="U8" s="73"/>
+      <c r="V8" s="73"/>
+      <c r="W8" s="73"/>
+      <c r="X8" s="74" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y8" s="74"/>
+      <c r="Z8" s="74"/>
+      <c r="AA8" s="74"/>
+      <c r="AB8" s="74"/>
+      <c r="AC8" s="74"/>
+      <c r="AD8" s="74"/>
+      <c r="AE8" s="74"/>
+      <c r="AF8" s="74"/>
+      <c r="AG8" s="74"/>
+      <c r="AH8" s="74"/>
+      <c r="AI8" s="74"/>
+      <c r="AJ8" s="74"/>
+      <c r="AK8" s="60"/>
+      <c r="AL8" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="Y8" s="88"/>
-      <c r="Z8" s="88"/>
-      <c r="AA8" s="88"/>
-      <c r="AB8" s="88"/>
-      <c r="AC8" s="88"/>
-      <c r="AD8" s="88"/>
-      <c r="AE8" s="88"/>
-      <c r="AF8" s="88"/>
-      <c r="AG8" s="88"/>
-      <c r="AH8" s="88"/>
-      <c r="AI8" s="88"/>
-      <c r="AJ8" s="88"/>
-      <c r="AK8" s="60"/>
-      <c r="AL8" s="68" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM8" s="68"/>
-      <c r="AN8" s="68"/>
-      <c r="AO8" s="68"/>
-      <c r="AP8" s="68"/>
-      <c r="AQ8" s="68"/>
-      <c r="AR8" s="68"/>
-      <c r="AS8" s="68"/>
-      <c r="AT8" s="68"/>
-      <c r="AU8" s="68"/>
-      <c r="AV8" s="68"/>
-      <c r="AW8" s="68"/>
-      <c r="AX8" s="68"/>
-      <c r="AY8" s="68"/>
+      <c r="AM8" s="81"/>
+      <c r="AN8" s="81"/>
+      <c r="AO8" s="81"/>
+      <c r="AP8" s="81"/>
+      <c r="AQ8" s="81"/>
+      <c r="AR8" s="81"/>
+      <c r="AS8" s="81"/>
+      <c r="AT8" s="81"/>
+      <c r="AU8" s="81"/>
+      <c r="AV8" s="81"/>
+      <c r="AW8" s="81"/>
+      <c r="AX8" s="81"/>
+      <c r="AY8" s="81"/>
       <c r="AZ8" s="18"/>
     </row>
     <row r="9" spans="1:52" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="22"/>
-      <c r="B9" s="82"/>
-      <c r="C9" s="82"/>
-      <c r="D9" s="82"/>
-      <c r="E9" s="82"/>
-      <c r="F9" s="82"/>
-      <c r="G9" s="82"/>
-      <c r="H9" s="82"/>
-      <c r="I9" s="82"/>
-      <c r="J9" s="84" t="s">
+      <c r="B9" s="66"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="84"/>
-      <c r="L9" s="84"/>
-      <c r="M9" s="84"/>
-      <c r="N9" s="84"/>
-      <c r="O9" s="84"/>
-      <c r="P9" s="85"/>
-      <c r="Q9" s="86" t="s">
+      <c r="K9" s="67"/>
+      <c r="L9" s="67"/>
+      <c r="M9" s="67"/>
+      <c r="N9" s="67"/>
+      <c r="O9" s="67"/>
+      <c r="P9" s="68"/>
+      <c r="Q9" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="R9" s="84"/>
-      <c r="S9" s="84"/>
-      <c r="T9" s="84"/>
-      <c r="U9" s="84"/>
-      <c r="V9" s="84"/>
-      <c r="W9" s="85"/>
-      <c r="X9" s="78" t="s">
-        <v>31</v>
-      </c>
-      <c r="Y9" s="79"/>
-      <c r="Z9" s="79"/>
-      <c r="AA9" s="79"/>
-      <c r="AB9" s="79"/>
-      <c r="AC9" s="79"/>
-      <c r="AD9" s="80"/>
-      <c r="AE9" s="78" t="s">
+      <c r="R9" s="67"/>
+      <c r="S9" s="67"/>
+      <c r="T9" s="67"/>
+      <c r="U9" s="67"/>
+      <c r="V9" s="67"/>
+      <c r="W9" s="68"/>
+      <c r="X9" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y9" s="71"/>
+      <c r="Z9" s="71"/>
+      <c r="AA9" s="71"/>
+      <c r="AB9" s="71"/>
+      <c r="AC9" s="71"/>
+      <c r="AD9" s="72"/>
+      <c r="AE9" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="AF9" s="79"/>
-      <c r="AG9" s="79"/>
-      <c r="AH9" s="79"/>
-      <c r="AI9" s="79"/>
-      <c r="AJ9" s="79"/>
-      <c r="AK9" s="80"/>
-      <c r="AL9" s="65" t="s">
+      <c r="AF9" s="71"/>
+      <c r="AG9" s="71"/>
+      <c r="AH9" s="71"/>
+      <c r="AI9" s="71"/>
+      <c r="AJ9" s="71"/>
+      <c r="AK9" s="72"/>
+      <c r="AL9" s="78" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM9" s="79"/>
+      <c r="AN9" s="79"/>
+      <c r="AO9" s="79"/>
+      <c r="AP9" s="79"/>
+      <c r="AQ9" s="79"/>
+      <c r="AR9" s="80"/>
+      <c r="AS9" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="AM9" s="66"/>
-      <c r="AN9" s="66"/>
-      <c r="AO9" s="66"/>
-      <c r="AP9" s="66"/>
-      <c r="AQ9" s="66"/>
-      <c r="AR9" s="67"/>
-      <c r="AS9" s="65" t="s">
-        <v>39</v>
-      </c>
-      <c r="AT9" s="66"/>
-      <c r="AU9" s="66"/>
-      <c r="AV9" s="66"/>
-      <c r="AW9" s="66"/>
-      <c r="AX9" s="66"/>
-      <c r="AY9" s="67"/>
+      <c r="AT9" s="79"/>
+      <c r="AU9" s="79"/>
+      <c r="AV9" s="79"/>
+      <c r="AW9" s="79"/>
+      <c r="AX9" s="79"/>
+      <c r="AY9" s="80"/>
       <c r="AZ9" s="22"/>
     </row>
     <row r="10" spans="1:52" s="55" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="22"/>
-      <c r="B10" s="82"/>
-      <c r="C10" s="82"/>
-      <c r="D10" s="82"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="82"/>
-      <c r="I10" s="82"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="66"/>
       <c r="J10" s="57">
         <v>10</v>
       </c>
@@ -1952,16 +1964,16 @@
     </row>
     <row r="11" spans="1:52" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="23"/>
-      <c r="B11" s="82"/>
-      <c r="C11" s="82"/>
-      <c r="D11" s="82"/>
-      <c r="E11" s="82"/>
-      <c r="F11" s="82"/>
-      <c r="G11" s="82"/>
-      <c r="H11" s="82"/>
-      <c r="I11" s="82"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="66"/>
+      <c r="I11" s="66"/>
       <c r="J11" s="57" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K11" s="24" t="s">
         <v>17</v>
@@ -1979,10 +1991,10 @@
         <v>21</v>
       </c>
       <c r="P11" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q11" s="57" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R11" s="24" t="s">
         <v>17</v>
@@ -2000,10 +2012,10 @@
         <v>21</v>
       </c>
       <c r="W11" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="X11" s="61" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y11" s="25" t="s">
         <v>17</v>
@@ -2021,10 +2033,10 @@
         <v>21</v>
       </c>
       <c r="AD11" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AE11" s="61" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AF11" s="25" t="s">
         <v>17</v>
@@ -2042,10 +2054,10 @@
         <v>21</v>
       </c>
       <c r="AK11" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AL11" s="64" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AM11" s="26" t="s">
         <v>17</v>
@@ -2063,10 +2075,10 @@
         <v>21</v>
       </c>
       <c r="AR11" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AS11" s="64" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AT11" s="26" t="s">
         <v>17</v>
@@ -2084,7 +2096,7 @@
         <v>21</v>
       </c>
       <c r="AY11" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AZ11" s="23"/>
     </row>
@@ -2152,7 +2164,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="D13" s="36" t="s">
         <v>24</v>
@@ -2164,14 +2176,14 @@
         <v>43965</v>
       </c>
       <c r="G13" s="38">
-        <f t="shared" ref="G13:G16" si="0">DAYS360(E13,F13)</f>
+        <f t="shared" ref="G13:G15" si="0">DAYS360(E13,F13)</f>
         <v>4</v>
       </c>
       <c r="H13" s="39">
         <v>0.2</v>
       </c>
       <c r="I13" s="39" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J13" s="42"/>
       <c r="K13" s="42"/>
@@ -2223,7 +2235,7 @@
         <v>1.2</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="36" t="s">
         <v>24</v>
@@ -2242,7 +2254,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="39" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J14" s="47"/>
       <c r="K14" s="47"/>
@@ -2288,47 +2300,47 @@
       <c r="AY14" s="52"/>
       <c r="AZ14" s="34"/>
     </row>
-    <row r="15" spans="1:52" s="62" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:52" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A15" s="34"/>
       <c r="B15" s="35">
         <v>1.3</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D15" s="36" t="s">
         <v>24</v>
       </c>
       <c r="E15" s="37">
-        <v>43964</v>
+        <v>43966</v>
       </c>
       <c r="F15" s="37">
-        <v>43969</v>
+        <v>43974</v>
       </c>
       <c r="G15" s="38">
-        <f t="shared" ref="G15" si="1">DAYS360(E15,F15)</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="H15" s="39">
         <v>0</v>
       </c>
       <c r="I15" s="39" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J15" s="47"/>
       <c r="K15" s="47"/>
       <c r="L15" s="48"/>
-      <c r="M15" s="47"/>
-      <c r="N15" s="48"/>
+      <c r="M15" s="49"/>
+      <c r="N15" s="49"/>
       <c r="O15" s="42"/>
       <c r="P15" s="42"/>
       <c r="Q15" s="42"/>
       <c r="R15" s="42"/>
-      <c r="S15" s="43"/>
-      <c r="T15" s="43"/>
-      <c r="U15" s="43"/>
-      <c r="V15" s="43"/>
-      <c r="W15" s="43"/>
+      <c r="S15" s="42"/>
+      <c r="T15" s="42"/>
+      <c r="U15" s="42"/>
+      <c r="V15" s="42"/>
+      <c r="W15" s="42"/>
       <c r="X15" s="50"/>
       <c r="Y15" s="50"/>
       <c r="Z15" s="50"/>
@@ -2359,274 +2371,257 @@
       <c r="AY15" s="52"/>
       <c r="AZ15" s="34"/>
     </row>
-    <row r="16" spans="1:52" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="34"/>
-      <c r="B16" s="35">
-        <v>1.3</v>
-      </c>
-      <c r="C16" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="36" t="s">
+    <row r="16" spans="1:52" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="18"/>
+      <c r="B16" s="27">
+        <v>2</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="33"/>
+      <c r="P16" s="33"/>
+      <c r="Q16" s="33"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="33"/>
+      <c r="T16" s="30"/>
+      <c r="U16" s="33"/>
+      <c r="V16" s="33"/>
+      <c r="W16" s="33"/>
+      <c r="X16" s="33"/>
+      <c r="Y16" s="33"/>
+      <c r="Z16" s="33"/>
+      <c r="AA16" s="33"/>
+      <c r="AB16" s="33"/>
+      <c r="AC16" s="33"/>
+      <c r="AD16" s="33"/>
+      <c r="AE16" s="33"/>
+      <c r="AF16" s="33"/>
+      <c r="AG16" s="33"/>
+      <c r="AH16" s="33"/>
+      <c r="AI16" s="33"/>
+      <c r="AJ16" s="33"/>
+      <c r="AK16" s="33"/>
+      <c r="AL16" s="33"/>
+      <c r="AM16" s="33"/>
+      <c r="AN16" s="33"/>
+      <c r="AO16" s="33"/>
+      <c r="AP16" s="33"/>
+      <c r="AQ16" s="33"/>
+      <c r="AR16" s="33"/>
+      <c r="AS16" s="33"/>
+      <c r="AT16" s="33"/>
+      <c r="AU16" s="33"/>
+      <c r="AV16" s="33"/>
+      <c r="AW16" s="33"/>
+      <c r="AX16" s="33"/>
+      <c r="AY16" s="33"/>
+      <c r="AZ16" s="18"/>
+    </row>
+    <row r="17" spans="1:52" s="55" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="18"/>
+      <c r="B17" s="35">
+        <v>2.1</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="37">
-        <v>43966</v>
-      </c>
-      <c r="F16" s="37">
-        <v>43974</v>
-      </c>
-      <c r="G16" s="38">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H16" s="39">
+      <c r="E17" s="37">
+        <v>43975</v>
+      </c>
+      <c r="F17" s="37">
+        <v>43978</v>
+      </c>
+      <c r="G17" s="38">
+        <v>4</v>
+      </c>
+      <c r="H17" s="39">
         <v>0</v>
       </c>
-      <c r="I16" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="J16" s="47"/>
-      <c r="K16" s="47"/>
-      <c r="L16" s="48"/>
-      <c r="M16" s="49"/>
-      <c r="N16" s="49"/>
-      <c r="O16" s="42"/>
-      <c r="P16" s="42"/>
-      <c r="Q16" s="42"/>
-      <c r="R16" s="42"/>
-      <c r="S16" s="42"/>
-      <c r="T16" s="42"/>
-      <c r="U16" s="42"/>
-      <c r="V16" s="42"/>
-      <c r="W16" s="42"/>
-      <c r="X16" s="50"/>
-      <c r="Y16" s="50"/>
-      <c r="Z16" s="50"/>
-      <c r="AA16" s="50"/>
-      <c r="AB16" s="50"/>
-      <c r="AC16" s="50"/>
-      <c r="AD16" s="50"/>
-      <c r="AE16" s="45"/>
-      <c r="AF16" s="45"/>
-      <c r="AG16" s="45"/>
-      <c r="AH16" s="45"/>
-      <c r="AI16" s="45"/>
-      <c r="AJ16" s="45"/>
-      <c r="AK16" s="45"/>
-      <c r="AL16" s="50"/>
-      <c r="AM16" s="50"/>
-      <c r="AN16" s="50"/>
-      <c r="AO16" s="50"/>
-      <c r="AP16" s="50"/>
-      <c r="AQ16" s="50"/>
-      <c r="AR16" s="50"/>
-      <c r="AS16" s="52"/>
-      <c r="AT16" s="52"/>
-      <c r="AU16" s="52"/>
-      <c r="AV16" s="52"/>
-      <c r="AW16" s="52"/>
-      <c r="AX16" s="52"/>
-      <c r="AY16" s="52"/>
-      <c r="AZ16" s="34"/>
-    </row>
-    <row r="17" spans="1:52" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="18"/>
-      <c r="B17" s="27">
-        <v>2</v>
-      </c>
-      <c r="C17" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="32"/>
-      <c r="O17" s="33"/>
-      <c r="P17" s="33"/>
-      <c r="Q17" s="33"/>
-      <c r="R17" s="30"/>
-      <c r="S17" s="33"/>
-      <c r="T17" s="30"/>
-      <c r="U17" s="33"/>
-      <c r="V17" s="33"/>
-      <c r="W17" s="33"/>
-      <c r="X17" s="33"/>
-      <c r="Y17" s="33"/>
-      <c r="Z17" s="33"/>
-      <c r="AA17" s="33"/>
-      <c r="AB17" s="33"/>
-      <c r="AC17" s="33"/>
-      <c r="AD17" s="33"/>
-      <c r="AE17" s="33"/>
-      <c r="AF17" s="33"/>
-      <c r="AG17" s="33"/>
-      <c r="AH17" s="33"/>
-      <c r="AI17" s="33"/>
-      <c r="AJ17" s="33"/>
-      <c r="AK17" s="33"/>
-      <c r="AL17" s="33"/>
-      <c r="AM17" s="33"/>
-      <c r="AN17" s="33"/>
-      <c r="AO17" s="33"/>
-      <c r="AP17" s="33"/>
-      <c r="AQ17" s="33"/>
-      <c r="AR17" s="33"/>
-      <c r="AS17" s="33"/>
-      <c r="AT17" s="33"/>
-      <c r="AU17" s="33"/>
-      <c r="AV17" s="33"/>
-      <c r="AW17" s="33"/>
-      <c r="AX17" s="33"/>
-      <c r="AY17" s="33"/>
+      <c r="I17" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="44"/>
+      <c r="N17" s="44"/>
+      <c r="O17" s="44"/>
+      <c r="P17" s="44"/>
+      <c r="Q17" s="43"/>
+      <c r="R17" s="43"/>
+      <c r="S17" s="43"/>
+      <c r="T17" s="43"/>
+      <c r="U17" s="43"/>
+      <c r="V17" s="43"/>
+      <c r="W17" s="43"/>
+      <c r="X17" s="53"/>
+      <c r="Y17" s="53"/>
+      <c r="Z17" s="53"/>
+      <c r="AA17" s="53"/>
+      <c r="AB17" s="44"/>
+      <c r="AC17" s="44"/>
+      <c r="AD17" s="44"/>
+      <c r="AE17" s="45"/>
+      <c r="AF17" s="45"/>
+      <c r="AG17" s="45"/>
+      <c r="AH17" s="45"/>
+      <c r="AI17" s="45"/>
+      <c r="AJ17" s="45"/>
+      <c r="AK17" s="45"/>
+      <c r="AL17" s="44"/>
+      <c r="AM17" s="44"/>
+      <c r="AN17" s="44"/>
+      <c r="AO17" s="44"/>
+      <c r="AP17" s="44"/>
+      <c r="AQ17" s="44"/>
+      <c r="AR17" s="44"/>
+      <c r="AS17" s="46"/>
+      <c r="AT17" s="46"/>
+      <c r="AU17" s="46"/>
+      <c r="AV17" s="46"/>
+      <c r="AW17" s="46"/>
+      <c r="AX17" s="46"/>
+      <c r="AY17" s="46"/>
       <c r="AZ17" s="18"/>
     </row>
-    <row r="18" spans="1:52" s="55" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="18"/>
+    <row r="18" spans="1:52" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="34"/>
       <c r="B18" s="35">
-        <v>2.1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="C18" s="36" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D18" s="36" t="s">
         <v>24</v>
       </c>
       <c r="E18" s="37">
-        <v>43975</v>
+        <v>43979</v>
       </c>
       <c r="F18" s="37">
-        <v>43978</v>
+        <v>43994</v>
       </c>
       <c r="G18" s="38">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H18" s="39">
         <v>0</v>
       </c>
       <c r="I18" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="44"/>
-      <c r="N18" s="44"/>
-      <c r="O18" s="44"/>
-      <c r="P18" s="44"/>
-      <c r="Q18" s="43"/>
-      <c r="R18" s="43"/>
-      <c r="S18" s="43"/>
-      <c r="T18" s="43"/>
-      <c r="U18" s="43"/>
-      <c r="V18" s="43"/>
-      <c r="W18" s="43"/>
-      <c r="X18" s="53"/>
-      <c r="Y18" s="53"/>
-      <c r="Z18" s="53"/>
-      <c r="AA18" s="53"/>
-      <c r="AB18" s="44"/>
-      <c r="AC18" s="44"/>
-      <c r="AD18" s="44"/>
-      <c r="AE18" s="45"/>
-      <c r="AF18" s="45"/>
-      <c r="AG18" s="45"/>
-      <c r="AH18" s="45"/>
-      <c r="AI18" s="45"/>
-      <c r="AJ18" s="45"/>
-      <c r="AK18" s="45"/>
-      <c r="AL18" s="44"/>
-      <c r="AM18" s="44"/>
-      <c r="AN18" s="44"/>
-      <c r="AO18" s="44"/>
-      <c r="AP18" s="44"/>
-      <c r="AQ18" s="44"/>
-      <c r="AR18" s="44"/>
-      <c r="AS18" s="46"/>
-      <c r="AT18" s="46"/>
-      <c r="AU18" s="46"/>
-      <c r="AV18" s="46"/>
-      <c r="AW18" s="46"/>
-      <c r="AX18" s="46"/>
-      <c r="AY18" s="46"/>
-      <c r="AZ18" s="18"/>
+        <v>46</v>
+      </c>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="49"/>
+      <c r="N18" s="49"/>
+      <c r="O18" s="50"/>
+      <c r="P18" s="50"/>
+      <c r="Q18" s="51"/>
+      <c r="R18" s="51"/>
+      <c r="S18" s="51"/>
+      <c r="T18" s="51"/>
+      <c r="U18" s="51"/>
+      <c r="V18" s="51"/>
+      <c r="W18" s="51"/>
+      <c r="X18" s="50"/>
+      <c r="Y18" s="50"/>
+      <c r="Z18" s="50"/>
+      <c r="AA18" s="50"/>
+      <c r="AB18" s="53"/>
+      <c r="AC18" s="53"/>
+      <c r="AD18" s="53"/>
+      <c r="AE18" s="53"/>
+      <c r="AF18" s="53"/>
+      <c r="AG18" s="53"/>
+      <c r="AH18" s="53"/>
+      <c r="AI18" s="53"/>
+      <c r="AJ18" s="53"/>
+      <c r="AK18" s="53"/>
+      <c r="AL18" s="63"/>
+      <c r="AM18" s="63"/>
+      <c r="AN18" s="63"/>
+      <c r="AO18" s="63"/>
+      <c r="AP18" s="63"/>
+      <c r="AQ18" s="63"/>
+      <c r="AR18" s="50"/>
+      <c r="AS18" s="52"/>
+      <c r="AT18" s="52"/>
+      <c r="AU18" s="52"/>
+      <c r="AV18" s="52"/>
+      <c r="AW18" s="52"/>
+      <c r="AX18" s="52"/>
+      <c r="AY18" s="52"/>
+      <c r="AZ18" s="34"/>
     </row>
-    <row r="19" spans="1:52" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="34"/>
-      <c r="B19" s="35">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="C19" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" s="37">
-        <v>43979</v>
-      </c>
-      <c r="F19" s="37">
-        <v>43994</v>
-      </c>
-      <c r="G19" s="38">
-        <v>0</v>
-      </c>
-      <c r="H19" s="39">
-        <v>0</v>
-      </c>
-      <c r="I19" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="J19" s="47"/>
-      <c r="K19" s="47"/>
-      <c r="L19" s="48"/>
-      <c r="M19" s="49"/>
-      <c r="N19" s="49"/>
-      <c r="O19" s="50"/>
-      <c r="P19" s="50"/>
-      <c r="Q19" s="51"/>
-      <c r="R19" s="51"/>
-      <c r="S19" s="51"/>
-      <c r="T19" s="51"/>
-      <c r="U19" s="51"/>
-      <c r="V19" s="51"/>
-      <c r="W19" s="51"/>
-      <c r="X19" s="50"/>
-      <c r="Y19" s="50"/>
-      <c r="Z19" s="50"/>
-      <c r="AA19" s="50"/>
-      <c r="AB19" s="53"/>
-      <c r="AC19" s="53"/>
-      <c r="AD19" s="53"/>
-      <c r="AE19" s="53"/>
-      <c r="AF19" s="53"/>
-      <c r="AG19" s="53"/>
-      <c r="AH19" s="53"/>
-      <c r="AI19" s="53"/>
-      <c r="AJ19" s="53"/>
-      <c r="AK19" s="53"/>
-      <c r="AL19" s="63"/>
-      <c r="AM19" s="63"/>
-      <c r="AN19" s="63"/>
-      <c r="AO19" s="63"/>
-      <c r="AP19" s="63"/>
-      <c r="AQ19" s="63"/>
-      <c r="AR19" s="50"/>
-      <c r="AS19" s="52"/>
-      <c r="AT19" s="52"/>
-      <c r="AU19" s="52"/>
-      <c r="AV19" s="52"/>
-      <c r="AW19" s="52"/>
-      <c r="AX19" s="52"/>
-      <c r="AY19" s="52"/>
-      <c r="AZ19" s="34"/>
+    <row r="19" spans="1:52" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
+      <c r="S19" s="18"/>
+      <c r="T19" s="18"/>
+      <c r="U19" s="18"/>
+      <c r="V19" s="18"/>
+      <c r="W19" s="18"/>
+      <c r="X19" s="18"/>
+      <c r="Y19" s="18"/>
+      <c r="Z19" s="18"/>
+      <c r="AA19" s="18"/>
+      <c r="AB19" s="18"/>
+      <c r="AC19" s="18"/>
+      <c r="AD19" s="18"/>
+      <c r="AE19" s="18"/>
+      <c r="AF19" s="18"/>
+      <c r="AG19" s="18"/>
+      <c r="AH19" s="18"/>
+      <c r="AI19" s="18"/>
+      <c r="AJ19" s="18"/>
+      <c r="AK19" s="18"/>
+      <c r="AL19" s="18"/>
+      <c r="AM19" s="18"/>
+      <c r="AN19" s="18"/>
+      <c r="AO19" s="18"/>
+      <c r="AP19" s="18"/>
+      <c r="AQ19" s="18"/>
+      <c r="AR19" s="18"/>
+      <c r="AS19" s="18"/>
+      <c r="AT19" s="18"/>
+      <c r="AU19" s="18"/>
+      <c r="AV19" s="18"/>
+      <c r="AW19" s="18"/>
+      <c r="AX19" s="18"/>
+      <c r="AY19" s="18"/>
+      <c r="AZ19" s="18"/>
     </row>
     <row r="20" spans="1:52" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="18"/>
@@ -2736,74 +2731,8 @@
       <c r="AY21" s="18"/>
       <c r="AZ21" s="18"/>
     </row>
-    <row r="22" spans="1:52" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="54"/>
-      <c r="H22" s="54"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="18"/>
-      <c r="T22" s="18"/>
-      <c r="U22" s="18"/>
-      <c r="V22" s="18"/>
-      <c r="W22" s="18"/>
-      <c r="X22" s="18"/>
-      <c r="Y22" s="18"/>
-      <c r="Z22" s="18"/>
-      <c r="AA22" s="18"/>
-      <c r="AB22" s="18"/>
-      <c r="AC22" s="18"/>
-      <c r="AD22" s="18"/>
-      <c r="AE22" s="18"/>
-      <c r="AF22" s="18"/>
-      <c r="AG22" s="18"/>
-      <c r="AH22" s="18"/>
-      <c r="AI22" s="18"/>
-      <c r="AJ22" s="18"/>
-      <c r="AK22" s="18"/>
-      <c r="AL22" s="18"/>
-      <c r="AM22" s="18"/>
-      <c r="AN22" s="18"/>
-      <c r="AO22" s="18"/>
-      <c r="AP22" s="18"/>
-      <c r="AQ22" s="18"/>
-      <c r="AR22" s="18"/>
-      <c r="AS22" s="18"/>
-      <c r="AT22" s="18"/>
-      <c r="AU22" s="18"/>
-      <c r="AV22" s="18"/>
-      <c r="AW22" s="18"/>
-      <c r="AX22" s="18"/>
-      <c r="AY22" s="18"/>
-      <c r="AZ22" s="18"/>
-    </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="I8:I11"/>
-    <mergeCell ref="J9:P9"/>
-    <mergeCell ref="Q9:W9"/>
-    <mergeCell ref="X9:AD9"/>
-    <mergeCell ref="J8:W8"/>
-    <mergeCell ref="X8:AJ8"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="G8:G11"/>
-    <mergeCell ref="F8:F11"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="E8:E11"/>
     <mergeCell ref="AL9:AR9"/>
     <mergeCell ref="AS9:AY9"/>
     <mergeCell ref="AL8:AY8"/>
@@ -2820,9 +2749,21 @@
     <mergeCell ref="C8:C11"/>
     <mergeCell ref="H8:H11"/>
     <mergeCell ref="B8:B11"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="G8:G11"/>
+    <mergeCell ref="F8:F11"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="I8:I11"/>
+    <mergeCell ref="J9:P9"/>
+    <mergeCell ref="Q9:W9"/>
+    <mergeCell ref="X9:AD9"/>
+    <mergeCell ref="J8:W8"/>
+    <mergeCell ref="X8:AJ8"/>
   </mergeCells>
   <phoneticPr fontId="28" type="noConversion"/>
-  <conditionalFormatting sqref="H18">
+  <conditionalFormatting sqref="H17">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -2832,7 +2773,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H18">
+  <conditionalFormatting sqref="H17">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -2842,47 +2783,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H15">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFFFFF"/>
-        <color rgb="FF57BB8A"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H15">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF57BB8A"/>
-        <color rgb="FFFFFFFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I15">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFFFFF"/>
-        <color rgb="FF57BB8A"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I15">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF57BB8A"/>
-        <color rgb="FFFFFFFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18">
+  <conditionalFormatting sqref="I17">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2892,7 +2793,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I18">
+  <conditionalFormatting sqref="I17">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2902,7 +2803,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H13:H14 H19 H16">
+  <conditionalFormatting sqref="H13:H15 H18">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -2912,7 +2813,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H13:H14 H19 H16">
+  <conditionalFormatting sqref="H13:H15 H18">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -2922,7 +2823,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I13:I14 I19 I16">
+  <conditionalFormatting sqref="I13:I15 I18">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
@@ -2932,7 +2833,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I13:I14 I19 I16">
+  <conditionalFormatting sqref="I13:I15 I18">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>